<commit_message>
Correction localsearch BUT instance02 not working
FUNZIONA, MA LA INSTANCE02 NO

variazioni:
- costVariation is double, not int
- tante altre cose
...
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Exams</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">Fill the green cells only!!! Do not change anything else!!! </t>
+  </si>
+  <si>
+    <t>bloccato</t>
+  </si>
+  <si>
+    <t>45 circa</t>
   </si>
 </sst>
 </file>
@@ -720,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -800,10 +806,12 @@
       <c r="G4" s="9">
         <v>157.03273300000001</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="23">
+        <v>157.91480000000001</v>
+      </c>
       <c r="J4" s="24">
         <f>100*(I4-G4)/G4</f>
-        <v>-100</v>
+        <v>0.56170900368906296</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -828,10 +836,12 @@
       <c r="G5" s="10">
         <v>34.708820000000003</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="3">
+      <c r="I5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="3" t="e">
         <f t="shared" ref="J5:J10" si="0">100*(I5-G5)/G5</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -856,10 +866,12 @@
       <c r="G6" s="10">
         <v>32.626666999999998</v>
       </c>
-      <c r="I6" s="22"/>
-      <c r="J6" s="3">
+      <c r="I6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="3" t="e">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -884,10 +896,12 @@
       <c r="G7" s="10">
         <v>7.7172020000000003</v>
       </c>
-      <c r="I7" s="22"/>
+      <c r="I7" s="22">
+        <v>10.5032</v>
+      </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>-99.999999999999986</v>
+        <v>36.101141320390468</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -912,10 +926,12 @@
       <c r="G8" s="10">
         <v>12.901103000000001</v>
       </c>
-      <c r="I8" s="22"/>
+      <c r="I8" s="22">
+        <v>19.07</v>
+      </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>47.816818453429903</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -940,10 +956,12 @@
       <c r="G9" s="10">
         <v>3.044578</v>
       </c>
-      <c r="I9" s="22"/>
+      <c r="I9" s="22">
+        <v>4.6900000000000004</v>
+      </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>54.044337179077047</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -968,37 +986,39 @@
       <c r="G10" s="12">
         <v>10.050300999999999</v>
       </c>
-      <c r="I10" s="22"/>
+      <c r="I10" s="22">
+        <v>12.2982</v>
+      </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>-100</v>
+        <v>22.366484347085731</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="4" t="e">
         <f>MIN(J4:J10)</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="4" t="e">
         <f>AVERAGE(J4:J10)</f>
-        <v>-100</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="4" t="e">
         <f>MAX(J4:J10)</f>
-        <v>-99.999999999999986</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reenhancing + best sol found
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -721,7 +721,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -832,11 +832,11 @@
         <v>34.708820000000003</v>
       </c>
       <c r="I5" s="22">
-        <v>42.79</v>
+        <v>39.9</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:J10" si="0">100*(I5-G5)/G5</f>
-        <v>23.282785182555891</v>
+        <v>14.956371320027577</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -862,11 +862,11 @@
         <v>32.626666999999998</v>
       </c>
       <c r="I6" s="22">
-        <v>40.17</v>
+        <v>39.14</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>23.12014586105288</v>
+        <v>19.963219044102797</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -892,11 +892,11 @@
         <v>7.7172020000000003</v>
       </c>
       <c r="I7" s="22">
-        <v>9.5830000000000002</v>
+        <v>9.15</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>24.177130519584686</v>
+        <v>18.566288662652603</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -982,11 +982,11 @@
         <v>10.050300999999999</v>
       </c>
       <c r="I10" s="22">
-        <v>10.96</v>
+        <v>10.957000000000001</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>9.0514602497975112</v>
+        <v>9.0216103975393533</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>20.800169213899522</v>
+        <v>18.353878872661141</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
arriving to the end..
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19100" windowHeight="9333"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12199" windowHeight="9333"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -922,11 +922,11 @@
         <v>12.901103000000001</v>
       </c>
       <c r="I8" s="22">
-        <v>16.739999999999998</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>29.756347189848785</v>
+        <v>29.213757924419333</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>18.353878872661141</v>
+        <v>18.276366120456938</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
miglioramenti e soluz migliori trovate
il nMaxDiIterazioni dentro generateFeasibleIndividual modificato a 300 mi permette di trovare un buon equilibrio
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Exams</t>
   </si>
@@ -73,6 +73,33 @@
   </si>
   <si>
     <t xml:space="preserve">Fill the green cells only!!! Do not change anything else!!! </t>
+  </si>
+  <si>
+    <t>inst02</t>
+  </si>
+  <si>
+    <t>300 iterations</t>
+  </si>
+  <si>
+    <t>inst06</t>
+  </si>
+  <si>
+    <t>7sec</t>
+  </si>
+  <si>
+    <t>subito</t>
+  </si>
+  <si>
+    <t>300-400 iterations</t>
+  </si>
+  <si>
+    <t>ez</t>
+  </si>
+  <si>
+    <t>inst05</t>
+  </si>
+  <si>
+    <t>6 sol in 29sec</t>
   </si>
 </sst>
 </file>
@@ -718,15 +745,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="15.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.75" customWidth="1"/>
     <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="5" max="5" width="11.625" customWidth="1"/>
@@ -802,11 +830,11 @@
         <v>157.03273300000001</v>
       </c>
       <c r="I4" s="23">
-        <v>157.4</v>
+        <v>157.40589198036</v>
       </c>
       <c r="J4" s="24">
         <f>100*(I4-G4)/G4</f>
-        <v>0.23387926388570096</v>
+        <v>0.23763133534712716</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -832,11 +860,11 @@
         <v>34.708820000000003</v>
       </c>
       <c r="I5" s="22">
-        <v>39.9</v>
+        <v>39.817215727948899</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ref="J5:J10" si="0">100*(I5-G5)/G5</f>
-        <v>14.956371320027577</v>
+        <v>14.71786055518135</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -861,12 +889,15 @@
       <c r="G6" s="10">
         <v>32.626666999999998</v>
       </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
       <c r="I6" s="22">
-        <v>39.14</v>
+        <v>39.146666666666597</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>19.963219044102797</v>
+        <v>19.983652227383814</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -891,12 +922,15 @@
       <c r="G7" s="10">
         <v>7.7172020000000003</v>
       </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
       <c r="I7" s="22">
-        <v>9.15</v>
+        <v>9.0325688073394499</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" si="0"/>
-        <v>18.566288662652603</v>
+        <v>17.044607713254745</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -922,11 +956,11 @@
         <v>12.901103000000001</v>
       </c>
       <c r="I8" s="22">
-        <v>16.670000000000002</v>
+        <v>15.322303234249301</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>29.213757924419333</v>
+        <v>18.767389379414301</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -952,11 +986,11 @@
         <v>3.044578</v>
       </c>
       <c r="I9" s="22">
-        <v>4.1399999999999997</v>
+        <v>4.00992194112668</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" si="0"/>
-        <v>35.979436230571189</v>
+        <v>31.706986686715858</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
@@ -982,11 +1016,11 @@
         <v>10.050300999999999</v>
       </c>
       <c r="I10" s="22">
-        <v>10.957000000000001</v>
+        <v>10.957137796670199</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>9.0216103975393533</v>
+        <v>9.0229814676217188</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -995,7 +1029,7 @@
       </c>
       <c r="J12" s="4">
         <f>MIN(J4:J10)</f>
-        <v>0.23387926388570096</v>
+        <v>0.23763133534712716</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1004,7 +1038,7 @@
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>18.276366120456938</v>
+        <v>15.925872766416989</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1013,7 +1047,7 @@
       </c>
       <c r="J14" s="4">
         <f>MAX(J4:J10)</f>
-        <v>35.979436230571189</v>
+        <v>31.706986686715858</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1027,6 +1061,36 @@
       <c r="H16" s="28"/>
       <c r="I16" s="29"/>
       <c r="J16" s="30"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ADDED SWAP TIMESLOT LOCAL SEARCH
migliora di molto le soluzioni
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -747,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -830,11 +830,11 @@
         <v>157.03273300000001</v>
       </c>
       <c r="I4" s="23">
-        <v>157.09819999999999</v>
+        <v>157.0736497545</v>
       </c>
       <c r="J4" s="24">
         <f>100*(I4-G4)/G4</f>
-        <v>4.1690034140833526E-2</v>
+        <v>2.605619460242654E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -890,11 +890,11 @@
         <v>32.626666999999998</v>
       </c>
       <c r="I6" s="22">
-        <v>39.012444000000002</v>
+        <v>37.638222222222197</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" si="0"/>
-        <v>19.572262775109714</v>
+        <v>15.360303956950919</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -950,11 +950,11 @@
         <v>12.901103000000001</v>
       </c>
       <c r="I8" s="22">
-        <v>15.130865999999999</v>
+        <v>15.0822583660497</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" si="0"/>
-        <v>17.283506689311746</v>
+        <v>16.906735540749494</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="J12" s="4">
         <f>MIN(J4:J10)</f>
-        <v>4.1690034140833526E-2</v>
+        <v>2.605619460242654E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1032,7 +1032,7 @@
       </c>
       <c r="J13" s="4">
         <f>AVERAGE(J4:J10)</f>
-        <v>14.067893029106228</v>
+        <v>13.410126771069161</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>